<commit_message>
home tests and search results
</commit_message>
<xml_diff>
--- a/src/test/java/data/ReservationDetails.xlsx
+++ b/src/test/java/data/ReservationDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NaghamStudy\Booking_Sumerage\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F3B9FC-DBE2-48D3-A796-BC3C58CAC247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6529567-1726-477E-8FE5-D33194E3145C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EC701116-1E54-4B5A-B3B9-7E3F23AAE39F}"/>
   </bookViews>
@@ -396,13 +396,13 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -412,10 +412,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>44652</v>
+        <v>45017</v>
       </c>
       <c r="C1" s="2">
-        <v>44665</v>
+        <v>45030</v>
       </c>
     </row>
   </sheetData>

</xml_diff>